<commit_message>
Cleaned up the curriculum
</commit_message>
<xml_diff>
--- a/KS1/Year-1.xlsx
+++ b/KS1/Year-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="11760" tabRatio="211"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="11760" tabRatio="23"/>
   </bookViews>
   <sheets>
     <sheet name="KS1" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="101">
   <si>
     <t>Lesson</t>
   </si>
@@ -64,21 +64,6 @@
 - I can make appropriate colour choices</t>
   </si>
   <si>
-    <t xml:space="preserve"> -I can choose appropriate paint tools and colours to recreate the work of an artist
-- I can say which tools were helpful and why
-- I know that different paint tools do different jobs</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -I can change the colour and brush sizes
-- I can make dots of colour on the page
-- I can use dots of colour to create a picture in the style of an artist on my own</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -I can explain that pictures can be made in lots of different ways
-- I can say whether I prefer painting using a computer or using paper
-- I can spot the differences between painting on a computer and on paper</t>
-  </si>
-  <si>
     <t>-To explain what a given command will do</t>
   </si>
   <si>
@@ -223,11 +208,6 @@
     <t>Project Requirements Specification (to be guided by the educator)</t>
   </si>
   <si>
-    <t>Learners should draw lines on a screen and explain which  tools I used
-Learners should make marks on a screen and explain which tools I used
-Learners should use the paint tools to draw a picture</t>
-  </si>
-  <si>
     <t>Learners should click and drag to make objects on a screen
 Learners should use a mouse to create a picture
 Learners should use a mouse to open a program</t>
@@ -300,21 +280,6 @@
 Learners should identify rules to keep us safe and healthy when we are using technology in and beyond the home</t>
   </si>
   <si>
-    <t>Learners should choose appropriate paint tools and colours to recreate the work of an artist
-Learners should say which tools were helpful and why
-Learners should different paint tools do different jobs</t>
-  </si>
-  <si>
-    <t>Learners should change the colour and brush sizes
-Learners should make dots of colour on the page
-Learners should use dots of colour to create a picture in the style of an artist on my own</t>
-  </si>
-  <si>
-    <t>Learners should explain that pictures can be made in lots of different ways
-Learners should say whether they prefer painting using a computer or using paper
-Learners should spot the differences between painting on a computer and on paper</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Learners should find which commands to move a sprite
 Learners should use commands to move a sprite</t>
@@ -361,12 +326,6 @@
   </si>
   <si>
     <t>Key Stage</t>
-  </si>
-  <si>
-    <t>To explain the reasons why given tools are used</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> To compare painting a picture on a computer and on paper</t>
   </si>
   <si>
     <t>To use an algorithm to create a program</t>
@@ -427,12 +386,6 @@
     <t>Bee-Bot                                                                                                                                         Blue-Bot,                                                                                                        or other fixed-movement floor robot</t>
   </si>
   <si>
-    <t>Digital painting</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> To use a computer to paint a picture</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">                                                                                                                               </t>
     </r>
@@ -589,12 +542,153 @@
   <si>
     <t>ScratchJr (Tablet)                                                                                                     Scratch Offline Editor (Desktop/Laptop)                                                                            scratch.mit.edu (Web)</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                                                                               </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Microsoft</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">aint (Offline)                                                                                            </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">paintz.app (Online)    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Learners should draw lines on a screen and explain which  tools  they used
+Learners should make marks on a screen and explain which tools they used
+Learners should use the paint tools to draw a picture</t>
+  </si>
+  <si>
+    <t>Design (DE)</t>
+  </si>
+  <si>
+    <t>Introduction to Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To create a sketch on a paper</t>
+  </si>
+  <si>
+    <t>To discuss the meaning of design as a communication tool.</t>
+  </si>
+  <si>
+    <t>Learners should discuss the meaning of design as a communication tool.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To design a basic picture using a Computer</t>
+  </si>
+  <si>
+    <t>Learners should design a basic picture using a Computer</t>
+  </si>
+  <si>
+    <t>Learners should create a sketch on a paper</t>
+  </si>
+  <si>
+    <t>I can discuss the meaning of design as a communication tool.</t>
+  </si>
+  <si>
+    <t>I can design a basic picture using the computer</t>
+  </si>
+  <si>
+    <t>I can create a sketch on a paper</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                                                                               </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="3" tint="0.14999847407452621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>White Drawing Paper</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="3" tint="0.14999847407452621"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -707,6 +801,20 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="3" tint="0.14999847407452621"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="3" tint="0.14999847407452621"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="11">
@@ -916,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1082,11 +1190,46 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1439,9 +1582,9 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1478,40 +1621,40 @@
     </row>
     <row r="2" spans="1:13" s="51" customFormat="1" ht="36.75" customHeight="1" thickBot="1">
       <c r="A2" s="52" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="43" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>39</v>
       </c>
       <c r="F2" s="43" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="43" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H2" s="43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I2" s="43" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K2" s="53" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L2" s="54" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M2" s="55"/>
     </row>
@@ -1523,13 +1666,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -1541,16 +1684,16 @@
         <v>1</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="K3" s="32" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M3" s="4">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(COUNTUNIQUE($C$3:C3))"),1)</f>
@@ -1565,13 +1708,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="6">
         <v>2</v>
@@ -1583,16 +1726,16 @@
         <v>2</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J4" s="40" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M4" s="8">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C4),2))"),1)</f>
@@ -1607,13 +1750,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F5" s="6">
         <v>3</v>
@@ -1625,13 +1768,13 @@
         <v>3</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J5" s="40" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="K5" s="33" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>2</v>
@@ -1649,13 +1792,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F6" s="14">
         <v>1</v>
@@ -1667,13 +1810,13 @@
         <v>1</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="41" t="s">
-        <v>95</v>
+        <v>29</v>
+      </c>
+      <c r="J6" s="59" t="s">
+        <v>87</v>
       </c>
       <c r="K6" s="34" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="L6" s="15" t="s">
         <v>6</v>
@@ -1691,13 +1834,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F7" s="6">
         <v>2</v>
@@ -1709,13 +1852,13 @@
         <v>2</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J7" s="41" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K7" s="33" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L7" s="7" t="s">
         <v>7</v>
@@ -1733,13 +1876,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F8" s="6">
         <v>3</v>
@@ -1751,13 +1894,13 @@
         <v>3</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J8" s="41" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="K8" s="33" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>8</v>
@@ -1775,13 +1918,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F9" s="14">
         <v>1</v>
@@ -1793,16 +1936,16 @@
         <v>1</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J9" s="44" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="M9" s="16">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C9),2))"),0)</f>
@@ -1817,13 +1960,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F10" s="6">
         <v>2</v>
@@ -1835,16 +1978,16 @@
         <v>2</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J10" s="44" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="K10" s="33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M10" s="17">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C10),2))"),0)</f>
@@ -1859,13 +2002,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F11" s="6">
         <v>3</v>
@@ -1877,16 +2020,16 @@
         <v>3</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J11" s="44" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="K11" s="33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M11" s="17">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C11),2))"),0)</f>
@@ -1901,13 +2044,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F12" s="6">
         <v>4</v>
@@ -1919,16 +2062,16 @@
         <v>1</v>
       </c>
       <c r="I12" s="56" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J12" s="44" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="K12" s="33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M12" s="17">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C12),2))"),0)</f>
@@ -1943,13 +2086,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F13" s="6">
         <v>5</v>
@@ -1961,16 +2104,16 @@
         <v>2</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J13" s="58" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="K13" s="33" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M13" s="17">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C13),2))"),0)</f>
@@ -1985,13 +2128,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F14" s="10">
         <v>6</v>
@@ -2003,16 +2146,16 @@
         <v>3</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J14" s="44" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="K14" s="35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M14" s="18">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C14),2))"),0)</f>
@@ -2027,13 +2170,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F15" s="6">
         <v>4</v>
@@ -2045,13 +2188,13 @@
         <v>1</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J15" s="40" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="K15" s="33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>3</v>
@@ -2069,13 +2212,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F16" s="6">
         <v>5</v>
@@ -2087,13 +2230,13 @@
         <v>2</v>
       </c>
       <c r="I16" s="29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J16" s="40" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="K16" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>4</v>
@@ -2111,13 +2254,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F17" s="10">
         <v>6</v>
@@ -2129,13 +2272,13 @@
         <v>3</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J17" s="40" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="K17" s="35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L17" s="11" t="s">
         <v>5</v>
@@ -2145,7 +2288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="70.5" customHeight="1">
+    <row r="18" spans="1:13" ht="87" customHeight="1">
       <c r="A18" s="27">
         <v>1</v>
       </c>
@@ -2153,13 +2296,13 @@
         <v>1</v>
       </c>
       <c r="C18" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>90</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>93</v>
       </c>
       <c r="F18" s="6">
         <v>1</v>
@@ -2171,23 +2314,23 @@
         <v>1</v>
       </c>
       <c r="I18" s="29" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="J18" s="41" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="M18" s="8">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C18),2))"),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="75" customHeight="1">
+    <row r="19" spans="1:13" ht="75.75" customHeight="1">
       <c r="A19" s="27">
         <v>1</v>
       </c>
@@ -2195,13 +2338,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>90</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>93</v>
       </c>
       <c r="F19" s="6">
         <v>2</v>
@@ -2216,13 +2359,13 @@
         <v>94</v>
       </c>
       <c r="J19" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="K19" s="33" t="s">
-        <v>70</v>
-      </c>
       <c r="L19" s="7" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="M19" s="8">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C19),2))"),1)</f>
@@ -2237,13 +2380,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>90</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>93</v>
       </c>
       <c r="F20" s="10">
         <v>3</v>
@@ -2255,16 +2398,16 @@
         <v>3</v>
       </c>
       <c r="I20" s="31" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="J20" s="41" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="K20" s="35" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="M20" s="12">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C20),2))"),1)</f>
@@ -2279,13 +2422,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F21" s="14">
         <v>1</v>
@@ -2297,16 +2440,16 @@
         <v>1</v>
       </c>
       <c r="I21" s="30" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J21" s="57" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="K21" s="34" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="M21" s="19">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C27),2))"),1)</f>
@@ -2321,13 +2464,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F22" s="6">
         <v>2</v>
@@ -2339,16 +2482,16 @@
         <v>2</v>
       </c>
       <c r="I22" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="J22" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="J22" s="57" t="s">
-        <v>97</v>
-      </c>
       <c r="K22" s="33" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="M22" s="8">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C28),2))"),1)</f>
@@ -2363,13 +2506,13 @@
         <v>1</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F23" s="6">
         <v>3</v>
@@ -2381,16 +2524,16 @@
         <v>3</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="J23" s="57" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="M23" s="8">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C29),2))"),1)</f>
@@ -2405,13 +2548,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F24" s="6">
         <v>4</v>
@@ -2423,16 +2566,16 @@
         <v>1</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="J24" s="57" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M24" s="17">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C36),2))"),0)</f>
@@ -2447,13 +2590,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F25" s="6">
         <v>5</v>
@@ -2465,16 +2608,16 @@
         <v>2</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="J25" s="57" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M25" s="17">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C37),2))"),0)</f>
@@ -2489,13 +2632,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F26" s="10">
         <v>6</v>
@@ -2507,16 +2650,16 @@
         <v>3</v>
       </c>
       <c r="I26" s="31" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="J26" s="57" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M26" s="18">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C38),2))"),0)</f>
@@ -2549,92 +2692,92 @@
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="M3:M26 B24:L26 C4:C26 B3:L5">
-    <cfRule type="expression" dxfId="17" priority="17">
+    <cfRule type="expression" dxfId="21" priority="17">
       <formula>$M3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M26 B24:L26 C4:C26 B3:L5">
-    <cfRule type="expression" dxfId="16" priority="19">
+    <cfRule type="expression" dxfId="20" priority="19">
       <formula>$M3=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:L23 J24:J26">
-    <cfRule type="expression" dxfId="15" priority="40">
+    <cfRule type="expression" dxfId="19" priority="40">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:L23 J24:J26">
-    <cfRule type="expression" dxfId="14" priority="41">
+    <cfRule type="expression" dxfId="18" priority="41">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:L17">
-    <cfRule type="expression" dxfId="13" priority="50">
+    <cfRule type="expression" dxfId="17" priority="50">
       <formula>$M6=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:L17">
-    <cfRule type="expression" dxfId="12" priority="52">
+    <cfRule type="expression" dxfId="16" priority="52">
       <formula>$M6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:L8">
-    <cfRule type="expression" dxfId="11" priority="54">
+    <cfRule type="expression" dxfId="15" priority="54">
       <formula>$M9=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:L8">
-    <cfRule type="expression" dxfId="10" priority="56">
+    <cfRule type="expression" dxfId="14" priority="56">
       <formula>$M9=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:L20">
-    <cfRule type="expression" dxfId="9" priority="58">
+    <cfRule type="expression" dxfId="13" priority="58">
       <formula>$M12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:L20">
-    <cfRule type="expression" dxfId="8" priority="60">
+    <cfRule type="expression" dxfId="12" priority="60">
       <formula>$M12=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:L14">
-    <cfRule type="expression" dxfId="7" priority="62">
+    <cfRule type="expression" dxfId="11" priority="62">
       <formula>$M15=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:L14">
-    <cfRule type="expression" dxfId="6" priority="64">
+    <cfRule type="expression" dxfId="10" priority="64">
       <formula>$M15=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J17">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>$M18=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J17">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>$M18=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J17">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>$M15=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J17">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>$M15=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:J20">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$M21=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:J20">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$M21=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>